<commit_message>
Working automatic excel to pdf converter using pywin32
</commit_message>
<xml_diff>
--- a/input/kopf.xlsx
+++ b/input/kopf.xlsx
@@ -19,15 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>Kopfhörer</t>
   </si>
   <si>
     <t>Tsschhau  saau</t>
-  </si>
-  <si>
-    <t>ffricckk</t>
   </si>
   <si>
     <t>Bewertung:</t>
@@ -623,7 +620,7 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,9 +651,7 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -667,56 +662,56 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="N2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J3" s="3"/>
       <c r="N3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O3" s="4">
         <v>1</v>
       </c>
       <c r="P3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="R3" s="4">
         <v>12</v>
@@ -727,7 +722,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="5">
         <v>6</v>
@@ -754,16 +749,16 @@
       </c>
       <c r="J4" s="3"/>
       <c r="N4" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O4" s="9">
         <v>2</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R4" s="9">
         <v>10</v>
@@ -774,7 +769,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="5">
         <v>6</v>
@@ -801,16 +796,16 @@
       </c>
       <c r="J5" s="3"/>
       <c r="N5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="8">
+        <v>3</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="O5" s="8">
-        <v>3</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="R5" s="8">
         <v>8</v>
@@ -819,12 +814,12 @@
         <v>70</v>
       </c>
       <c r="W5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="5">
         <v>6</v>
@@ -851,16 +846,16 @@
       </c>
       <c r="J6" s="3"/>
       <c r="N6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="6">
+        <v>4</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="O6" s="6">
-        <v>4</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="R6" s="6">
         <v>6</v>
@@ -871,7 +866,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="10">
         <v>7</v>
@@ -898,16 +893,16 @@
       </c>
       <c r="J7" s="3"/>
       <c r="N7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" s="7">
+        <v>5</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="O7" s="7">
-        <v>5</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q7" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="R7" s="7">
         <v>4</v>
@@ -918,7 +913,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="7">
         <v>5</v>
@@ -945,16 +940,16 @@
       </c>
       <c r="J8" s="3"/>
       <c r="N8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O8" s="5">
         <v>6</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R8" s="5">
         <v>2</v>
@@ -965,7 +960,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="7">
         <v>5</v>
@@ -992,16 +987,16 @@
       </c>
       <c r="J9" s="3"/>
       <c r="N9" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O9" s="10">
         <v>7</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q9" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R9" s="10">
         <v>0</v>
@@ -1028,7 +1023,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="5">
         <v>6</v>
@@ -1063,7 +1058,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="5">
         <v>6</v>
@@ -1099,7 +1094,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="8">
         <v>3</v>
@@ -1135,7 +1130,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="6">
         <v>4</v>
@@ -1169,7 +1164,7 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="5">
         <v>6</v>
@@ -1205,7 +1200,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="5">
         <v>6</v>
@@ -1241,7 +1236,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="5">
         <v>6</v>
@@ -1506,9 +1501,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Arial"&amp;1 &amp;K000000INTERNAL#</oddHeader>
+    <oddHeader>&amp;L&amp;"Arial"&amp;8&amp;K000000INTERNAL&amp;1#_x000D_&amp;"Calibri"&amp;11&amp;K000000&amp;"Arial"&amp;1 &amp;K000000INTERNAL#</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Automatic module download, window support, bug fix
</commit_message>
<xml_diff>
--- a/input/kopf.xlsx
+++ b/input/kopf.xlsx
@@ -19,13 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
-  <si>
-    <t>Kopfhörer</t>
-  </si>
-  <si>
-    <t>Tsschhau  saau</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>Bewertung:</t>
   </si>
@@ -142,6 +136,9 @@
   </si>
   <si>
     <t>Devialet Gemini</t>
+  </si>
+  <si>
+    <t>Example</t>
   </si>
 </sst>
 </file>
@@ -620,7 +617,7 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,15 +641,13 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C1"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -664,56 +659,56 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="N2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J3" s="3"/>
       <c r="N3" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="O3" s="4">
         <v>1</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="R3" s="4">
         <v>12</v>
@@ -724,7 +719,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="5">
         <v>6</v>
@@ -751,16 +746,16 @@
       </c>
       <c r="J4" s="3"/>
       <c r="N4" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="O4" s="9">
         <v>2</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="R4" s="9">
         <v>10</v>
@@ -771,7 +766,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="5">
         <v>6</v>
@@ -798,16 +793,16 @@
       </c>
       <c r="J5" s="3"/>
       <c r="N5" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O5" s="8">
         <v>3</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="R5" s="8">
         <v>8</v>
@@ -816,12 +811,12 @@
         <v>70</v>
       </c>
       <c r="W5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="5">
         <v>6</v>
@@ -848,16 +843,16 @@
       </c>
       <c r="J6" s="3"/>
       <c r="N6" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O6" s="6">
         <v>4</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="R6" s="6">
         <v>6</v>
@@ -868,7 +863,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="10">
         <v>7</v>
@@ -895,16 +890,16 @@
       </c>
       <c r="J7" s="3"/>
       <c r="N7" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O7" s="7">
         <v>5</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="R7" s="7">
         <v>4</v>
@@ -915,7 +910,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="7">
         <v>5</v>
@@ -942,16 +937,16 @@
       </c>
       <c r="J8" s="3"/>
       <c r="N8" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O8" s="5">
         <v>6</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R8" s="5">
         <v>2</v>
@@ -962,7 +957,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B9" s="7">
         <v>5</v>
@@ -989,16 +984,16 @@
       </c>
       <c r="J9" s="3"/>
       <c r="N9" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O9" s="10">
         <v>7</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="Q9" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="R9" s="10">
         <v>0</v>
@@ -1025,7 +1020,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="5">
         <v>6</v>
@@ -1060,7 +1055,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="5">
         <v>6</v>
@@ -1096,7 +1091,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" s="8">
         <v>3</v>
@@ -1132,7 +1127,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B14" s="6">
         <v>4</v>
@@ -1166,7 +1161,7 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="5">
         <v>6</v>
@@ -1202,7 +1197,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" s="5">
         <v>6</v>
@@ -1238,7 +1233,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="5">
         <v>6</v>

</xml_diff>